<commit_message>
Deploying to main from @ electrified/rcbus-ymf262@ebfbf4c0577dcc72f495dd32770ceaaf84c5ee7e 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/rcbus-ymf262-bom.xlsx
+++ b/BoM/Positional/rcbus-ymf262-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="287">
   <si>
     <t>Row</t>
   </si>
@@ -182,7 +182,7 @@
     <t>0.9500</t>
   </si>
   <si>
-    <t>GND,Net-(U3-AOUT)</t>
+    <t>Net-(U3-AOUT),GND</t>
   </si>
   <si>
     <t>Default</t>
@@ -230,519 +230,516 @@
     <t>90.0000</t>
   </si>
   <si>
-    <t>GND,/AUDIO_CH2</t>
+    <t>/AUDIO_CH2,GND</t>
+  </si>
+  <si>
+    <t>AUDIO_CH2,GND</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>C17 C18</t>
+  </si>
+  <si>
+    <t>3.9nF</t>
+  </si>
+  <si>
+    <t>-18.2780</t>
+  </si>
+  <si>
+    <t>10.3180</t>
+  </si>
+  <si>
+    <t>Net-(C17-Pad1),GND</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>-26.3606</t>
+  </si>
+  <si>
+    <t>-16.0501</t>
+  </si>
+  <si>
+    <t>0.0000</t>
+  </si>
+  <si>
+    <t>VCC,GND</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>C1 C3 C6 C7 C12</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>rcbus-ymf262(5)</t>
+  </si>
+  <si>
+    <t>-50.1905</t>
+  </si>
+  <si>
+    <t>-26.2820</t>
+  </si>
+  <si>
+    <t>180.0000</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Polarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>C_Polarized_Small</t>
+  </si>
+  <si>
+    <t>C15 C16</t>
+  </si>
+  <si>
+    <t>10uf</t>
+  </si>
+  <si>
+    <t>-28.5280</t>
+  </si>
+  <si>
+    <t>/L,Net-(C15-Pad2)</t>
+  </si>
+  <si>
+    <t>L,Net-(C15-Pad2)</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>C4 C5</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>C_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>-15.3606</t>
+  </si>
+  <si>
+    <t>4.1000</t>
+  </si>
+  <si>
+    <t>1.8000</t>
+  </si>
+  <si>
+    <t>GND,Net-(C3-Pad1)</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>-44.0280</t>
+  </si>
+  <si>
+    <t>-0.0445</t>
+  </si>
+  <si>
+    <t>Net-(U3-CV),GND</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>Connector_Audio</t>
+  </si>
+  <si>
+    <t>CON1</t>
+  </si>
+  <si>
+    <t>SJ1-3523N</t>
+  </si>
+  <si>
+    <t>Headphone_Jack_3.5mm_5_pin</t>
+  </si>
+  <si>
+    <t>electrified</t>
+  </si>
+  <si>
+    <t>electrified:Headphone_Jack_3.5mm_5_pin</t>
+  </si>
+  <si>
+    <t>-11.4590</t>
+  </si>
+  <si>
+    <t>6.2230</t>
+  </si>
+  <si>
+    <t>THT</t>
+  </si>
+  <si>
+    <t>9.3500</t>
+  </si>
+  <si>
+    <t>11.8000</t>
+  </si>
+  <si>
+    <t>,Net-(C18-Pad1),Net-(C17-Pad1),GND</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x06, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x06_Odd_Even</t>
+  </si>
+  <si>
+    <t>Connector_Generic</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>BASE ADDRESS</t>
+  </si>
+  <si>
+    <t>PinHeader_2x06_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm:PinHeader_2x06_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>-95.5280</t>
+  </si>
+  <si>
+    <t>-24.8420</t>
+  </si>
+  <si>
+    <t>4.2400</t>
+  </si>
+  <si>
+    <t>14.4000</t>
+  </si>
+  <si>
+    <t>Net-(JP1-Pin_7),Net-(JP1-Pin_11),Net-(JP1-Pin_3),Net-(JP1-Pin_9),VCC,Net-(JP1-Pin_5),Net-(JP1-Pin_1)</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>33uH</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
+  </si>
+  <si>
+    <t>Inductor_SMD</t>
+  </si>
+  <si>
+    <t>Inductor_SMD:L_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
+  </si>
+  <si>
+    <t>-9.8606</t>
+  </si>
+  <si>
+    <t>+5VA,Net-(C3-Pad1)</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>BLM18PG221SN1D</t>
+  </si>
+  <si>
+    <t>-23.7356</t>
+  </si>
+  <si>
+    <t>-11.0501</t>
+  </si>
+  <si>
+    <t>VCC,Net-(C3-Pad1)</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x39, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_01x39</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>RC2014 BUS</t>
+  </si>
+  <si>
+    <t>PinHeader_1x39_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>electrified:PinHeader_1x39_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>-98.5280</t>
+  </si>
+  <si>
+    <t>-31.6820</t>
+  </si>
+  <si>
+    <t>1.7000</t>
+  </si>
+  <si>
+    <t>98.2200</t>
+  </si>
+  <si>
+    <t>unconnected-(P1-Pin_5-Pad5),/~{RD},/D7,unconnected-(P1-Pin_37-Pad37),/D6,unconnected-(P1-Pin_8-Pad8),/D1,unconnected-(P1-Pin_36-Pad36),/A2,unconnected-(P1-Pin_1-Pad1),unconnected-(P1-Pin_23-Pad23),unconnected-(P1-Pin_6-Pad6),unconnected-(P1-Pin_19-Pad19),unconnected-(P1-Pin_2-Pad2),unconnected-(P1-Pin_7-Pad7),/~{INT},unconnected-(P1-Pin_35-Pad35),/A5,/A3,/A1,/A6,/A4,/D0,unconnected-(P1-Pin_4-Pad4),unconnected-(P1-Pin_3-Pad3),/D3,unconnected-(P1-Pin_39-Pad39),/A0,/~{IORQ},/D5,unconnected-(P1-Pin_38-Pad38),/D2,unconnected-(P1-Pin_21-Pad21),/~{WR},VCC,GND,/D4,/~{RESET},/A7</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>R_0603_1608Metric_Pad0.98x0.95mm_HandSolder</t>
+  </si>
+  <si>
+    <t>Resistor_SMD</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_0603_1608Metric_Pad0.98x0.95mm_HandSolder</t>
+  </si>
+  <si>
+    <t>-38.2780</t>
+  </si>
+  <si>
+    <t>-0.0945</t>
+  </si>
+  <si>
+    <t>Net-(U3-SWIN),Net-(U4B--)</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>R10 R11</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>-23.5280</t>
+  </si>
+  <si>
+    <t>10.0680</t>
+  </si>
+  <si>
+    <t>Net-(C15-Pad2),Net-(C17-Pad1)</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Resistor, small symbol</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R1 R2 R3 R4 R5 R6</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>rcbus-ymf262(6)</t>
+  </si>
+  <si>
+    <t>-86.3905</t>
+  </si>
+  <si>
+    <t>-12.1520</t>
+  </si>
+  <si>
+    <t>Net-(JP1-Pin_11),GND</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>R8 R9</t>
+  </si>
+  <si>
+    <t>15k</t>
+  </si>
+  <si>
+    <t>-37.7780</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>8-bit magnitude comparator</t>
+  </si>
+  <si>
+    <t>74HCT688</t>
+  </si>
+  <si>
+    <t>74xx</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>Package_SO</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
+  </si>
+  <si>
+    <t>Package_SO:SOIC-20W_7.5x12.8mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>-73.9330</t>
+  </si>
+  <si>
+    <t>-20.5320</t>
+  </si>
+  <si>
+    <t>11.3500</t>
+  </si>
+  <si>
+    <t>12.0300</t>
+  </si>
+  <si>
+    <t>/A6,/A4,Net-(JP1-Pin_7),/~{CS},/A2,Net-(JP1-Pin_11),Net-(JP1-Pin_3),Net-(JP1-Pin_9),VCC,/~{IORQ},GND,Net-(JP1-Pin_5),/A5,Net-(JP1-Pin_1),/A3,/A7</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Quad Low-Noise JFET-Input Operational Amplifiers, DIP-14/SOIC-14</t>
+  </si>
+  <si>
+    <t>TL074</t>
+  </si>
+  <si>
+    <t>Amplifier_Operational</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
+  </si>
+  <si>
+    <t>Package_SO:SOIC-14_3.9x8.7mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>-41.3905</t>
+  </si>
+  <si>
+    <t>5.8180</t>
+  </si>
+  <si>
+    <t>6.9000</t>
+  </si>
+  <si>
+    <t>8.2200</t>
+  </si>
+  <si>
+    <t>Net-(U4D--),+5VA,/R,Net-(U3-CV),Net-(U4C--),/AUDIO_CH1,Net-(U3-AOUT),Net-(U3-MP),Net-(U4B--),/L,/AUDIO_CH2,GND</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>YAC512</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>Package_SO:SOP-16_4.55x10.3mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>-41.5280</t>
+  </si>
+  <si>
+    <t>-8.6820</t>
+  </si>
+  <si>
+    <t>8.1000</t>
+  </si>
+  <si>
+    <t>9.4900</t>
+  </si>
+  <si>
+    <t>Net-(U3-MP),/DAC_CLK,+5VA,Net-(U3-SWIN),/SMPAC,/AUDIO_CH1,Net-(U3-CV),/SMPBD,Net-(U3-AOUT),GND,unconnected-(U3-TST2-Pad15),/DOAB,/AUDIO_CH2</t>
   </si>
   <si>
     <t>AUDIO_CH2</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>C17 C18</t>
-  </si>
-  <si>
-    <t>3.9nF</t>
-  </si>
-  <si>
-    <t>-18.2780</t>
-  </si>
-  <si>
-    <t>10.3180</t>
-  </si>
-  <si>
-    <t>Net-(C17-Pad1),GND</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>-26.3606</t>
-  </si>
-  <si>
-    <t>-16.0501</t>
-  </si>
-  <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>GND,VCC</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>C1 C3 C6 C7 C12</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>rcbus-ymf262(5)</t>
-  </si>
-  <si>
-    <t>-50.1905</t>
-  </si>
-  <si>
-    <t>-26.2820</t>
-  </si>
-  <si>
-    <t>180.0000</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Polarized capacitor, small symbol</t>
-  </si>
-  <si>
-    <t>C_Polarized_Small</t>
-  </si>
-  <si>
-    <t>C15 C16</t>
-  </si>
-  <si>
-    <t>10uf</t>
-  </si>
-  <si>
-    <t>-28.5280</t>
-  </si>
-  <si>
-    <t>Net-(C15-Pad2),/L</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>C4 C5</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>C_1206_3216Metric</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:C_1206_3216Metric</t>
-  </si>
-  <si>
-    <t>-15.3606</t>
-  </si>
-  <si>
-    <t>4.1000</t>
-  </si>
-  <si>
-    <t>1.8000</t>
-  </si>
-  <si>
-    <t>Net-(C3-Pad1),GND</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>-44.0280</t>
-  </si>
-  <si>
-    <t>-0.0445</t>
-  </si>
-  <si>
-    <t>GND,Net-(U3-CV)</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>Connector_Audio</t>
-  </si>
-  <si>
-    <t>CON1</t>
-  </si>
-  <si>
-    <t>SJ1-3523N</t>
-  </si>
-  <si>
-    <t>Headphone_Jack_3.5mm_5_pin</t>
-  </si>
-  <si>
-    <t>electrified</t>
-  </si>
-  <si>
-    <t>electrified:Headphone_Jack_3.5mm_5_pin</t>
-  </si>
-  <si>
-    <t>-11.4590</t>
-  </si>
-  <si>
-    <t>6.2230</t>
-  </si>
-  <si>
-    <t>THT</t>
-  </si>
-  <si>
-    <t>9.3500</t>
-  </si>
-  <si>
-    <t>11.8000</t>
-  </si>
-  <si>
-    <t>,GND,Net-(C18-Pad1),Net-(C17-Pad1)</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x06, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x06_Odd_Even</t>
-  </si>
-  <si>
-    <t>Connector_Generic</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>BASE ADDRESS</t>
-  </si>
-  <si>
-    <t>PinHeader_2x06_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Connector_PinHeader_2.54mm</t>
-  </si>
-  <si>
-    <t>Connector_PinHeader_2.54mm:PinHeader_2x06_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>-95.5280</t>
-  </si>
-  <si>
-    <t>-24.8420</t>
-  </si>
-  <si>
-    <t>4.2400</t>
-  </si>
-  <si>
-    <t>14.4000</t>
-  </si>
-  <si>
-    <t>Net-(JP1-Pin_9),Net-(JP1-Pin_3),Net-(JP1-Pin_11),VCC,Net-(JP1-Pin_7),Net-(JP1-Pin_1),Net-(JP1-Pin_5)</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>33uH</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
-  </si>
-  <si>
-    <t>Inductor_SMD</t>
-  </si>
-  <si>
-    <t>Inductor_SMD:L_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
-  </si>
-  <si>
-    <t>-9.8606</t>
-  </si>
-  <si>
-    <t>Net-(C3-Pad1),+5VA</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>BLM18PG221SN1D</t>
-  </si>
-  <si>
-    <t>-23.7356</t>
-  </si>
-  <si>
-    <t>-11.0501</t>
-  </si>
-  <si>
-    <t>Net-(C3-Pad1),VCC</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x39, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_01x39</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>RC2014 BUS</t>
-  </si>
-  <si>
-    <t>PinHeader_1x39_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>electrified:PinHeader_1x39_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>-98.5280</t>
-  </si>
-  <si>
-    <t>-31.6820</t>
-  </si>
-  <si>
-    <t>1.7000</t>
-  </si>
-  <si>
-    <t>98.2200</t>
-  </si>
-  <si>
-    <t>/D6,/~{RESET},/A6,unconnected-(P1-Pin_5-Pad5),/A2,unconnected-(P1-Pin_21-Pad21),unconnected-(P1-Pin_8-Pad8),unconnected-(P1-Pin_4-Pad4),/~{RD},/~{IORQ},unconnected-(P1-Pin_35-Pad35),/A0,/D4,/A5,GND,VCC,unconnected-(P1-Pin_23-Pad23),unconnected-(P1-Pin_36-Pad36),unconnected-(P1-Pin_1-Pad1),unconnected-(P1-Pin_7-Pad7),/D2,unconnected-(P1-Pin_19-Pad19),/A3,/A1,unconnected-(P1-Pin_6-Pad6),/D5,unconnected-(P1-Pin_2-Pad2),unconnected-(P1-Pin_38-Pad38),unconnected-(P1-Pin_37-Pad37),unconnected-(P1-Pin_39-Pad39),/~{INT},/A4,/D3,/D0,unconnected-(P1-Pin_3-Pad3),/~{WR},/A7,/D7,/D1</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>R_0603_1608Metric_Pad0.98x0.95mm_HandSolder</t>
-  </si>
-  <si>
-    <t>Resistor_SMD</t>
-  </si>
-  <si>
-    <t>Resistor_SMD:R_0603_1608Metric_Pad0.98x0.95mm_HandSolder</t>
-  </si>
-  <si>
-    <t>-38.2780</t>
-  </si>
-  <si>
-    <t>-0.0945</t>
-  </si>
-  <si>
-    <t>Net-(U4B--),Net-(U3-SWIN)</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>R10 R11</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>-23.5280</t>
-  </si>
-  <si>
-    <t>10.0680</t>
-  </si>
-  <si>
-    <t>Net-(C15-Pad2),Net-(C17-Pad1)</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R1 R2 R3 R4 R5 R6</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>rcbus-ymf262(6)</t>
-  </si>
-  <si>
-    <t>-86.3905</t>
-  </si>
-  <si>
-    <t>-12.1520</t>
-  </si>
-  <si>
-    <t>Net-(JP1-Pin_11),GND</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>R8 R9</t>
-  </si>
-  <si>
-    <t>15k</t>
-  </si>
-  <si>
-    <t>-37.7780</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>8-bit magnitude comparator</t>
-  </si>
-  <si>
-    <t>74HCT688</t>
-  </si>
-  <si>
-    <t>74xx</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>Package_SO</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
-  </si>
-  <si>
-    <t>Package_SO:SOIC-20W_7.5x12.8mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>-73.9330</t>
-  </si>
-  <si>
-    <t>-20.5320</t>
-  </si>
-  <si>
-    <t>11.3500</t>
-  </si>
-  <si>
-    <t>12.0300</t>
-  </si>
-  <si>
-    <t>/A4,Net-(JP1-Pin_9),/A3,/A5,GND,Net-(JP1-Pin_3),/A6,Net-(JP1-Pin_7),/A2,VCC,/A7,Net-(JP1-Pin_11),/~{CS},Net-(JP1-Pin_1),Net-(JP1-Pin_5),/~{IORQ}</t>
-  </si>
-  <si>
-    <t>~{IORQ}</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Quad Low-Noise JFET-Input Operational Amplifiers, DIP-14/SOIC-14</t>
-  </si>
-  <si>
-    <t>TL074</t>
-  </si>
-  <si>
-    <t>Amplifier_Operational</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
-  </si>
-  <si>
-    <t>Package_SO:SOIC-14_3.9x8.7mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>-41.3905</t>
-  </si>
-  <si>
-    <t>5.8180</t>
-  </si>
-  <si>
-    <t>6.9000</t>
-  </si>
-  <si>
-    <t>8.2200</t>
-  </si>
-  <si>
-    <t>Net-(U4B--),Net-(U4C--),/R,GND,/L,Net-(U3-AOUT),/AUDIO_CH2,Net-(U3-CV),/AUDIO_CH1,Net-(U4D--),Net-(U3-MP),+5VA</t>
-  </si>
-  <si>
-    <t>AUDIO_CH1,Net-(U4D--),Net-(U3-MP),+5VA</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>YAC512</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>Package_SO:SOP-16_4.55x10.3mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>-41.5280</t>
-  </si>
-  <si>
-    <t>-8.6820</t>
-  </si>
-  <si>
-    <t>8.1000</t>
-  </si>
-  <si>
-    <t>9.4900</t>
-  </si>
-  <si>
-    <t>/SMPBD,/SMPAC,GND,unconnected-(U3-TST2-Pad15),Net-(U3-AOUT),/AUDIO_CH2,Net-(U3-CV),/AUDIO_CH1,/DAC_CLK,/DOAB,Net-(U3-MP),+5VA,Net-(U3-SWIN)</t>
-  </si>
-  <si>
-    <t>DOAB,Net-(U3-MP),+5VA,Net-(U3-SWIN)</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
@@ -770,10 +767,10 @@
     <t>14.5200</t>
   </si>
   <si>
-    <t>/~{RESET},/~{RD},/A0,/D4,/CLK,unconnected-(U2-~{IRQ}-Pad2),GND,VCC,/DAC_CLK,/~{CS},/D1,/D2,/SMPAC,/A1,/D5,unconnected-(U2-TEST-Pad9),/SMPBD,unconnected-(U2-DOCD-Pad22),/D3,/D0,/~{WR},/D7,/DOAB,/D6</t>
-  </si>
-  <si>
-    <t>D6</t>
+    <t>unconnected-(U2-TEST-Pad9),/~{RD},/D7,/D6,/D1,unconnected-(U2-~{IRQ}-Pad2),unconnected-(U2-DOCD-Pad22),/A1,/D0,/CLK,/~{CS},/SMPAC,/D3,/A0,/D5,/D2,/DOAB,/~{WR},/DAC_CLK,/SMPBD,VCC,GND,/D4,/~{RESET}</t>
+  </si>
+  <si>
+    <t>~{RESET}</t>
   </si>
   <si>
     <t>23</t>
@@ -812,10 +809,10 @@
     <t>9.2200</t>
   </si>
   <si>
-    <t>unconnected-(X1-EN-Pad1),GND,VCC,/CLK</t>
-  </si>
-  <si>
-    <t>CLK</t>
+    <t>VCC,GND,/CLK,unconnected-(X1-EN-Pad1)</t>
+  </si>
+  <si>
+    <t>CLK,unconnected-(X1-EN-Pad1)</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -1423,7 +1420,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1457,13 +1454,13 @@
     </row>
     <row r="2" spans="1:32">
       <c r="C2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>268</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F2" s="3">
         <v>23</v>
@@ -1471,41 +1468,41 @@
     </row>
     <row r="3" spans="1:32">
       <c r="C3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="C4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:32">
       <c r="C5" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>274</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1513,13 +1510,13 @@
     </row>
     <row r="6" spans="1:32">
       <c r="C6" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F6" s="3">
         <v>39</v>
@@ -2709,22 +2706,22 @@
         <v>144</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>32</v>
@@ -2754,10 +2751,10 @@
         <v>44</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="T20" s="11" t="s">
         <v>82</v>
@@ -2787,10 +2784,10 @@
         <v>143</v>
       </c>
       <c r="AC20" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AD20" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AE20" s="10" t="s">
         <v>55</v>
@@ -2801,28 +2798,28 @@
     </row>
     <row r="21" spans="1:32">
       <c r="A21" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>144</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>32</v>
@@ -2852,13 +2849,13 @@
         <v>44</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="U21" s="7" t="s">
         <v>91</v>
@@ -2882,13 +2879,13 @@
         <v>53</v>
       </c>
       <c r="AB21" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AC21" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AD21" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AE21" s="6" t="s">
         <v>55</v>
@@ -2897,27 +2894,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="180" customHeight="1">
+    <row r="22" spans="1:32" ht="165" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>132</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>121</v>
@@ -2950,13 +2947,13 @@
         <v>44</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S22" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T22" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U22" s="11" t="s">
         <v>69</v>
@@ -2974,19 +2971,19 @@
         <v>51</v>
       </c>
       <c r="Z22" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AA22" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AB22" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AC22" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AD22" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AE22" s="10" t="s">
         <v>55</v>
@@ -2997,28 +2994,28 @@
     </row>
     <row r="23" spans="1:32">
       <c r="A23" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>32</v>
@@ -3048,13 +3045,13 @@
         <v>44</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>69</v>
@@ -3078,13 +3075,13 @@
         <v>53</v>
       </c>
       <c r="AB23" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AC23" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AD23" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AE23" s="6" t="s">
         <v>55</v>
@@ -3095,28 +3092,28 @@
     </row>
     <row r="24" spans="1:32">
       <c r="A24" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>56</v>
@@ -3146,13 +3143,13 @@
         <v>44</v>
       </c>
       <c r="R24" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="S24" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="U24" s="11" t="s">
         <v>48</v>
@@ -3176,13 +3173,13 @@
         <v>53</v>
       </c>
       <c r="AB24" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AC24" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AD24" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AE24" s="10" t="s">
         <v>55</v>
@@ -3193,28 +3190,28 @@
     </row>
     <row r="25" spans="1:32">
       <c r="A25" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>85</v>
@@ -3232,7 +3229,7 @@
         <v>42</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O25" s="8" t="s">
         <v>44</v>
@@ -3244,13 +3241,13 @@
         <v>44</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="U25" s="7" t="s">
         <v>91</v>
@@ -3274,13 +3271,13 @@
         <v>53</v>
       </c>
       <c r="AB25" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AD25" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AE25" s="6" t="s">
         <v>55</v>
@@ -3291,28 +3288,28 @@
     </row>
     <row r="26" spans="1:32">
       <c r="A26" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>56</v>
@@ -3342,10 +3339,10 @@
         <v>44</v>
       </c>
       <c r="R26" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="S26" s="11" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="T26" s="11" t="s">
         <v>62</v>
@@ -3372,7 +3369,7 @@
         <v>53</v>
       </c>
       <c r="AB26" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AC26" s="10" t="s">
         <v>63</v>
@@ -3389,28 +3386,28 @@
     </row>
     <row r="27" spans="1:32" ht="45" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>203</v>
-      </c>
       <c r="G27" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>32</v>
@@ -3422,7 +3419,7 @@
         <v>40</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M27" s="7" t="s">
         <v>42</v>
@@ -3440,13 +3437,13 @@
         <v>44</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="S27" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="U27" s="7" t="s">
         <v>69</v>
@@ -3464,19 +3461,19 @@
         <v>51</v>
       </c>
       <c r="Z27" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AA27" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AB27" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AC27" s="6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AD27" s="6" t="s">
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="AE27" s="6" t="s">
         <v>55</v>
@@ -3485,7 +3482,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:32" ht="45" customHeight="1">
+    <row r="28" spans="1:32" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
         <v>216</v>
       </c>
@@ -3508,7 +3505,7 @@
         <v>221</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>32</v>
@@ -3574,7 +3571,7 @@
         <v>228</v>
       </c>
       <c r="AD28" s="10" t="s">
-        <v>229</v>
+        <v>71</v>
       </c>
       <c r="AE28" s="10" t="s">
         <v>55</v>
@@ -3585,28 +3582,28 @@
     </row>
     <row r="29" spans="1:32" ht="45" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>121</v>
       </c>
       <c r="E29" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="G29" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>233</v>
-      </c>
       <c r="H29" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>32</v>
@@ -3636,13 +3633,13 @@
         <v>44</v>
       </c>
       <c r="R29" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="S29" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="S29" s="7" t="s">
+      <c r="T29" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="T29" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="U29" s="7" t="s">
         <v>69</v>
@@ -3660,19 +3657,19 @@
         <v>51</v>
       </c>
       <c r="Z29" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA29" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="AA29" s="7" t="s">
+      <c r="AB29" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC29" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="AB29" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="AC29" s="6" t="s">
+      <c r="AD29" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="AD29" s="6" t="s">
-        <v>240</v>
       </c>
       <c r="AE29" s="6" t="s">
         <v>55</v>
@@ -3683,28 +3680,28 @@
     </row>
     <row r="30" spans="1:32" ht="60" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>242</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>121</v>
       </c>
       <c r="E30" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>244</v>
-      </c>
       <c r="H30" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>32</v>
@@ -3734,13 +3731,13 @@
         <v>44</v>
       </c>
       <c r="R30" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="S30" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="S30" s="11" t="s">
+      <c r="T30" s="11" t="s">
         <v>246</v>
-      </c>
-      <c r="T30" s="11" t="s">
-        <v>247</v>
       </c>
       <c r="U30" s="11" t="s">
         <v>69</v>
@@ -3758,19 +3755,19 @@
         <v>51</v>
       </c>
       <c r="Z30" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA30" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="AA30" s="11" t="s">
+      <c r="AB30" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC30" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="AB30" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="AC30" s="10" t="s">
+      <c r="AD30" s="10" t="s">
         <v>250</v>
-      </c>
-      <c r="AD30" s="10" t="s">
-        <v>251</v>
       </c>
       <c r="AE30" s="10" t="s">
         <v>55</v>
@@ -3781,25 +3778,25 @@
     </row>
     <row r="31" spans="1:32">
       <c r="A31" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>254</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>121</v>
       </c>
       <c r="E31" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="G31" s="7" t="s">
         <v>256</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>257</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>121</v>
@@ -3814,7 +3811,7 @@
         <v>40</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M31" s="7" t="s">
         <v>42</v>
@@ -3832,13 +3829,13 @@
         <v>44</v>
       </c>
       <c r="R31" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="S31" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="S31" s="7" t="s">
+      <c r="T31" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="T31" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="U31" s="7" t="s">
         <v>83</v>
@@ -3856,19 +3853,19 @@
         <v>51</v>
       </c>
       <c r="Z31" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA31" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="AA31" s="7" t="s">
+      <c r="AB31" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC31" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="AB31" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="AC31" s="6" t="s">
+      <c r="AD31" s="6" t="s">
         <v>264</v>
-      </c>
-      <c r="AD31" s="6" t="s">
-        <v>265</v>
       </c>
       <c r="AE31" s="6" t="s">
         <v>55</v>
@@ -3900,27 +3897,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-ymf262@50cde1917e7c56b94f7a4ad0cab6380bee82dbe2 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/rcbus-ymf262-bom.xlsx
+++ b/BoM/Positional/rcbus-ymf262-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="283">
   <si>
     <t>Row</t>
   </si>
@@ -182,7 +182,7 @@
     <t>0.9500</t>
   </si>
   <si>
-    <t>GND,Net-(U3-AOUT)</t>
+    <t>Net-(U3-AOUT),GND</t>
   </si>
   <si>
     <t>Default</t>
@@ -209,237 +209,240 @@
     <t>12.8180</t>
   </si>
   <si>
-    <t>Net-(U4C--),/L</t>
+    <t>/L,Net-(U4C--)</t>
+  </si>
+  <si>
+    <t>L,Net-(U4C--)</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C9 C10</t>
+  </si>
+  <si>
+    <t>2.7nf</t>
+  </si>
+  <si>
+    <t>-40.0280</t>
+  </si>
+  <si>
+    <t>90.0000</t>
+  </si>
+  <si>
+    <t>/AUDIO_CH2,GND</t>
+  </si>
+  <si>
+    <t>AUDIO_CH2,GND</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>C17 C18</t>
+  </si>
+  <si>
+    <t>3.9nF</t>
+  </si>
+  <si>
+    <t>-18.2780</t>
+  </si>
+  <si>
+    <t>10.3180</t>
+  </si>
+  <si>
+    <t>Net-(C17-Pad1),GND</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>-79.0280</t>
+  </si>
+  <si>
+    <t>-5.6820</t>
+  </si>
+  <si>
+    <t>0.0000</t>
+  </si>
+  <si>
+    <t>VCC,GND</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>C1 C3 C6 C7 C12 C19</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>rcbus-ymf262(6)</t>
+  </si>
+  <si>
+    <t>-49.2780</t>
+  </si>
+  <si>
+    <t>-25.4320</t>
+  </si>
+  <si>
+    <t>180.0000</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Polarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>C_Polarized_Small</t>
+  </si>
+  <si>
+    <t>C8 C15 C16</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>rcbus-ymf262(3)</t>
+  </si>
+  <si>
+    <t>-44.0280</t>
+  </si>
+  <si>
+    <t>-0.0445</t>
+  </si>
+  <si>
+    <t>Net-(U3-CV),GND</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>C4 C5</t>
+  </si>
+  <si>
+    <t>C_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>-68.0280</t>
+  </si>
+  <si>
+    <t>4.1000</t>
+  </si>
+  <si>
+    <t>1.8000</t>
+  </si>
+  <si>
+    <t>Net-(C3-Pad1),GND</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>Connector_Audio</t>
+  </si>
+  <si>
+    <t>CON1</t>
+  </si>
+  <si>
+    <t>SJ1-3523N</t>
+  </si>
+  <si>
+    <t>Headphone_Jack_3.5mm_5_pin</t>
+  </si>
+  <si>
+    <t>electrified</t>
+  </si>
+  <si>
+    <t>electrified:Headphone_Jack_3.5mm_5_pin</t>
+  </si>
+  <si>
+    <t>-11.4590</t>
+  </si>
+  <si>
+    <t>6.2230</t>
+  </si>
+  <si>
+    <t>THT</t>
+  </si>
+  <si>
+    <t>9.3500</t>
+  </si>
+  <si>
+    <t>11.8000</t>
+  </si>
+  <si>
+    <t>,GND,Net-(C18-Pad1),Net-(C17-Pad1)</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x06, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x06_Odd_Even</t>
+  </si>
+  <si>
+    <t>Connector_Generic</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>BASE ADDRESS</t>
+  </si>
+  <si>
+    <t>PinHeader_2x06_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm:PinHeader_2x06_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>-95.5280</t>
+  </si>
+  <si>
+    <t>-24.8420</t>
+  </si>
+  <si>
+    <t>4.2400</t>
+  </si>
+  <si>
+    <t>14.4000</t>
+  </si>
+  <si>
+    <t>Net-(JP1-Pin_3),Net-(JP1-Pin_7),Net-(JP1-Pin_9),Net-(JP1-Pin_11),VCC,Net-(JP1-Pin_5),Net-(JP1-Pin_1)</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Inductor</t>
   </si>
   <si>
     <t>L</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>C9 C10</t>
-  </si>
-  <si>
-    <t>2.7nf</t>
-  </si>
-  <si>
-    <t>-40.0280</t>
-  </si>
-  <si>
-    <t>90.0000</t>
-  </si>
-  <si>
-    <t>/AUDIO_CH2,GND</t>
-  </si>
-  <si>
-    <t>AUDIO_CH2,GND</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>C17 C18</t>
-  </si>
-  <si>
-    <t>3.9nF</t>
-  </si>
-  <si>
-    <t>-18.2780</t>
-  </si>
-  <si>
-    <t>10.3180</t>
-  </si>
-  <si>
-    <t>GND,Net-(C17-Pad1)</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>-79.0280</t>
-  </si>
-  <si>
-    <t>-5.6820</t>
-  </si>
-  <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>GND,VCC</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>C1 C3 C6 C7 C12 C19</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>rcbus-ymf262(6)</t>
-  </si>
-  <si>
-    <t>-49.2780</t>
-  </si>
-  <si>
-    <t>-25.4320</t>
-  </si>
-  <si>
-    <t>180.0000</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Polarized capacitor, small symbol</t>
-  </si>
-  <si>
-    <t>C_Polarized_Small</t>
-  </si>
-  <si>
-    <t>C8 C15 C16</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>rcbus-ymf262(3)</t>
-  </si>
-  <si>
-    <t>-44.0280</t>
-  </si>
-  <si>
-    <t>-0.0445</t>
-  </si>
-  <si>
-    <t>GND,Net-(U3-CV)</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>C4 C5</t>
-  </si>
-  <si>
-    <t>C_1206_3216Metric</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:C_1206_3216Metric</t>
-  </si>
-  <si>
-    <t>-68.0280</t>
-  </si>
-  <si>
-    <t>4.1000</t>
-  </si>
-  <si>
-    <t>1.8000</t>
-  </si>
-  <si>
-    <t>GND,Net-(C3-Pad1)</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>Connector_Audio</t>
-  </si>
-  <si>
-    <t>CON1</t>
-  </si>
-  <si>
-    <t>SJ1-3523N</t>
-  </si>
-  <si>
-    <t>Headphone_Jack_3.5mm_5_pin</t>
-  </si>
-  <si>
-    <t>electrified</t>
-  </si>
-  <si>
-    <t>electrified:Headphone_Jack_3.5mm_5_pin</t>
-  </si>
-  <si>
-    <t>-11.4590</t>
-  </si>
-  <si>
-    <t>6.2230</t>
-  </si>
-  <si>
-    <t>THT</t>
-  </si>
-  <si>
-    <t>9.3500</t>
-  </si>
-  <si>
-    <t>11.8000</t>
-  </si>
-  <si>
-    <t>,GND,Net-(C18-Pad1),Net-(C17-Pad1)</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x06, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x06_Odd_Even</t>
-  </si>
-  <si>
-    <t>Connector_Generic</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>BASE ADDRESS</t>
-  </si>
-  <si>
-    <t>PinHeader_2x06_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Connector_PinHeader_2.54mm</t>
-  </si>
-  <si>
-    <t>Connector_PinHeader_2.54mm:PinHeader_2x06_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>-95.5280</t>
-  </si>
-  <si>
-    <t>-24.8420</t>
-  </si>
-  <si>
-    <t>4.2400</t>
-  </si>
-  <si>
-    <t>14.4000</t>
-  </si>
-  <si>
-    <t>Net-(JP1-Pin_11),Net-(JP1-Pin_9),VCC,Net-(JP1-Pin_3),Net-(JP1-Pin_1),Net-(JP1-Pin_5),Net-(JP1-Pin_7)</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
     <t>L2</t>
   </si>
   <si>
@@ -458,7 +461,7 @@
     <t>-62.5280</t>
   </si>
   <si>
-    <t>+5VA,Net-(C3-Pad1)</t>
+    <t>Net-(C3-Pad1),+5VA</t>
   </si>
   <si>
     <t>12</t>
@@ -476,7 +479,7 @@
     <t>-0.6820</t>
   </si>
   <si>
-    <t>VCC,Net-(C3-Pad1)</t>
+    <t>Net-(C3-Pad1),VCC</t>
   </si>
   <si>
     <t>13</t>
@@ -512,10 +515,10 @@
     <t>98.2200</t>
   </si>
   <si>
-    <t>/D5,unconnected-(P1-Pin_38-Pad38),/D3,unconnected-(P1-Pin_37-Pad37),unconnected-(P1-Pin_21-Pad21),/A1,unconnected-(P1-Pin_39-Pad39),unconnected-(P1-Pin_2-Pad2),/~{WR},/D2,/D6,/D0,/~{IORQ},/~{RESET},unconnected-(P1-Pin_4-Pad4),/A3,unconnected-(P1-Pin_6-Pad6),/D4,/A7,/D7,unconnected-(P1-Pin_8-Pad8),/A5,/~{RD},unconnected-(P1-Pin_23-Pad23),GND,VCC,unconnected-(P1-Pin_1-Pad1),/A6,/A0,unconnected-(P1-Pin_19-Pad19),/D1,unconnected-(P1-Pin_5-Pad5),unconnected-(P1-Pin_35-Pad35),unconnected-(P1-Pin_7-Pad7),/A2,unconnected-(P1-Pin_3-Pad3),/A4,/~{INT},unconnected-(P1-Pin_36-Pad36)</t>
-  </si>
-  <si>
-    <t>~{INT},unconnected-(P1-Pin_36-Pad36)</t>
+    <t>/~{INT},/A3,/A2,unconnected-(P1-Pin_36-Pad36),/~{IORQ},unconnected-(P1-Pin_23-Pad23),/D5,/A0,unconnected-(P1-Pin_39-Pad39),unconnected-(P1-Pin_8-Pad8),/D4,unconnected-(P1-Pin_19-Pad19),unconnected-(P1-Pin_3-Pad3),unconnected-(P1-Pin_37-Pad37),VCC,unconnected-(P1-Pin_5-Pad5),unconnected-(P1-Pin_4-Pad4),/D2,GND,/D1,/A5,unconnected-(P1-Pin_21-Pad21),/~{WR},/~{RD},/D0,unconnected-(P1-Pin_35-Pad35),/A4,unconnected-(P1-Pin_2-Pad2),unconnected-(P1-Pin_1-Pad1),/A6,unconnected-(P1-Pin_6-Pad6),/D3,unconnected-(P1-Pin_38-Pad38),/A7,/A1,/~{RESET},/D6,unconnected-(P1-Pin_7-Pad7),/D7</t>
+  </si>
+  <si>
+    <t>D7</t>
   </si>
   <si>
     <t>14</t>
@@ -548,7 +551,7 @@
     <t>-0.0945</t>
   </si>
   <si>
-    <t>Net-(U3-SWIN),Net-(U4B--)</t>
+    <t>Net-(U4B--),Net-(U3-SWIN)</t>
   </si>
   <si>
     <t>15</t>
@@ -566,7 +569,7 @@
     <t>10.0680</t>
   </si>
   <si>
-    <t>Net-(C15-Pad2),Net-(C17-Pad1)</t>
+    <t>Net-(C17-Pad1),Net-(C15-Pad2)</t>
   </si>
   <si>
     <t>16</t>
@@ -590,7 +593,7 @@
     <t>-12.1520</t>
   </si>
   <si>
-    <t>GND,Net-(JP1-Pin_11)</t>
+    <t>Net-(JP1-Pin_11),GND</t>
   </si>
   <si>
     <t>17</t>
@@ -605,12 +608,6 @@
     <t>-37.7780</t>
   </si>
   <si>
-    <t>/L,Net-(U4C--)</t>
-  </si>
-  <si>
-    <t>L,Net-(U4C--)</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -650,10 +647,10 @@
     <t>12.0300</t>
   </si>
   <si>
-    <t>Net-(JP1-Pin_11),Net-(JP1-Pin_9),GND,VCC,/~{IORQ},Net-(JP1-Pin_3),/A2,Net-(JP1-Pin_1),/A4,Net-(JP1-Pin_7),/A6,Net-(JP1-Pin_5),/A3,/A7,/~{CS},/A5</t>
-  </si>
-  <si>
-    <t>A5</t>
+    <t>/A3,Net-(JP1-Pin_3),/A2,Net-(JP1-Pin_7),GND,Net-(JP1-Pin_9),Net-(JP1-Pin_11),/A5,/~{IORQ},/A7,/~{CS},VCC,/A4,Net-(JP1-Pin_5),/A6,Net-(JP1-Pin_1)</t>
+  </si>
+  <si>
+    <t>A6,Net-(JP1-Pin_1)</t>
   </si>
   <si>
     <t>19</t>
@@ -692,10 +689,10 @@
     <t>8.2200</t>
   </si>
   <si>
-    <t>/AUDIO_CH2,Net-(U3-CV),/R,Net-(U4C--),+5VA,Net-(U4B--),GND,Net-(U3-MP),/L,Net-(U4D--),/AUDIO_CH1,Net-(U3-AOUT)</t>
-  </si>
-  <si>
-    <t>AUDIO_CH1,Net-(U3-AOUT)</t>
+    <t>Net-(U4B--),Net-(U4C--),+5VA,GND,Net-(U3-CV),/AUDIO_CH2,Net-(U4D--),/R,Net-(U3-AOUT),/L,Net-(U3-MP),/AUDIO_CH1</t>
+  </si>
+  <si>
+    <t>AUDIO_CH1</t>
   </si>
   <si>
     <t>20</t>
@@ -725,10 +722,10 @@
     <t>9.4900</t>
   </si>
   <si>
-    <t>/AUDIO_CH2,/SMPAC,Net-(U3-CV),+5VA,GND,/SMPBD,Net-(U3-MP),/DAC_CLK,Net-(U3-SWIN),unconnected-(U3-TST2-Pad15),/AUDIO_CH1,Net-(U3-AOUT),/DOAB</t>
-  </si>
-  <si>
-    <t>DOAB</t>
+    <t>Net-(U3-SWIN),/SMPAC,GND,/DOAB,+5VA,/DAC_CLK,/AUDIO_CH2,unconnected-(U3-TST2-Pad15),Net-(U3-CV),/SMPBD,Net-(U3-AOUT),/AUDIO_CH1,Net-(U3-MP)</t>
+  </si>
+  <si>
+    <t>AUDIO_CH1,Net-(U3-MP)</t>
   </si>
   <si>
     <t>21</t>
@@ -758,7 +755,7 @@
     <t>14.5200</t>
   </si>
   <si>
-    <t>/D5,unconnected-(U2-TEST-Pad9),/D3,/SMPBD,/A1,unconnected-(U2-DOCD-Pad22),/DAC_CLK,/~{WR},/D2,/D6,/CLK,/SMPAC,/D0,/~{RESET},/D4,/D7,/~{RD},GND,VCC,/A0,/D1,/~{CS},unconnected-(U2-~{IRQ}-Pad2),/DOAB</t>
+    <t>/DOAB,/D5,/A0,/SMPAC,/DAC_CLK,/D4,unconnected-(U2-~{IRQ}-Pad2),unconnected-(U2-DOCD-Pad22),VCC,unconnected-(U2-TEST-Pad9),/D2,GND,/D1,/~{WR},/~{RD},/D0,/SMPBD,/CLK,/D3,/A1,/~{RESET},/~{CS},/D6,/D7</t>
   </si>
   <si>
     <t>22</t>
@@ -800,10 +797,10 @@
     <t>6.0000</t>
   </si>
   <si>
-    <t>/CLK,GND,VCC</t>
-  </si>
-  <si>
-    <t>CLK,GND,VCC</t>
+    <t>/CLK,VCC,GND</t>
+  </si>
+  <si>
+    <t>CLK,VCC,GND</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -1411,7 +1408,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1445,13 +1442,13 @@
     </row>
     <row r="2" spans="1:32">
       <c r="C2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>264</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F2" s="3">
         <v>22</v>
@@ -1459,41 +1456,41 @@
     </row>
     <row r="3" spans="1:32">
       <c r="C3" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>266</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="C4" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>268</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:32">
       <c r="C5" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1501,13 +1498,13 @@
     </row>
     <row r="6" spans="1:32">
       <c r="C6" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F6" s="3">
         <v>40</v>
@@ -2599,22 +2596,22 @@
         <v>139</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>32</v>
@@ -2644,10 +2641,10 @@
         <v>44</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="T19" s="7" t="s">
         <v>82</v>
@@ -2677,10 +2674,10 @@
         <v>138</v>
       </c>
       <c r="AC19" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AD19" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AE19" s="6" t="s">
         <v>55</v>
@@ -2691,28 +2688,28 @@
     </row>
     <row r="20" spans="1:32">
       <c r="A20" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>139</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I20" s="9" t="s">
         <v>32</v>
@@ -2742,13 +2739,13 @@
         <v>44</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="T20" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="U20" s="11" t="s">
         <v>91</v>
@@ -2772,13 +2769,13 @@
         <v>53</v>
       </c>
       <c r="AB20" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AC20" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AD20" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AE20" s="10" t="s">
         <v>55</v>
@@ -2789,25 +2786,25 @@
     </row>
     <row r="21" spans="1:32" ht="180" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>127</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>116</v>
@@ -2840,13 +2837,13 @@
         <v>44</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="U21" s="7" t="s">
         <v>69</v>
@@ -2864,19 +2861,19 @@
         <v>51</v>
       </c>
       <c r="Z21" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AA21" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AB21" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AC21" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AD21" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AE21" s="6" t="s">
         <v>55</v>
@@ -2887,28 +2884,28 @@
     </row>
     <row r="22" spans="1:32">
       <c r="A22" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>32</v>
@@ -2938,13 +2935,13 @@
         <v>44</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S22" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="T22" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="U22" s="11" t="s">
         <v>69</v>
@@ -2968,13 +2965,13 @@
         <v>53</v>
       </c>
       <c r="AB22" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AC22" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AD22" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AE22" s="10" t="s">
         <v>55</v>
@@ -2985,28 +2982,28 @@
     </row>
     <row r="23" spans="1:32">
       <c r="A23" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>56</v>
@@ -3036,13 +3033,13 @@
         <v>44</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>48</v>
@@ -3066,13 +3063,13 @@
         <v>53</v>
       </c>
       <c r="AB23" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AC23" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AD23" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AE23" s="6" t="s">
         <v>55</v>
@@ -3083,28 +3080,28 @@
     </row>
     <row r="24" spans="1:32">
       <c r="A24" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>85</v>
@@ -3134,13 +3131,13 @@
         <v>44</v>
       </c>
       <c r="R24" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S24" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="U24" s="11" t="s">
         <v>83</v>
@@ -3164,13 +3161,13 @@
         <v>53</v>
       </c>
       <c r="AB24" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AC24" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AD24" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AE24" s="10" t="s">
         <v>55</v>
@@ -3181,28 +3178,28 @@
     </row>
     <row r="25" spans="1:32">
       <c r="A25" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>56</v>
@@ -3232,10 +3229,10 @@
         <v>44</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="T25" s="7" t="s">
         <v>62</v>
@@ -3262,13 +3259,13 @@
         <v>53</v>
       </c>
       <c r="AB25" s="6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>195</v>
+        <v>63</v>
       </c>
       <c r="AD25" s="6" t="s">
-        <v>196</v>
+        <v>64</v>
       </c>
       <c r="AE25" s="6" t="s">
         <v>55</v>
@@ -3279,28 +3276,28 @@
     </row>
     <row r="26" spans="1:32" ht="45" customHeight="1">
       <c r="A26" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="F26" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="G26" s="11" t="s">
+      <c r="H26" s="11" t="s">
         <v>202</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>32</v>
@@ -3312,7 +3309,7 @@
         <v>40</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M26" s="11" t="s">
         <v>42</v>
@@ -3330,13 +3327,13 @@
         <v>44</v>
       </c>
       <c r="R26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="S26" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="S26" s="11" t="s">
+      <c r="T26" s="11" t="s">
         <v>206</v>
-      </c>
-      <c r="T26" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="U26" s="11" t="s">
         <v>69</v>
@@ -3354,19 +3351,19 @@
         <v>51</v>
       </c>
       <c r="Z26" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA26" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="AA26" s="11" t="s">
+      <c r="AB26" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC26" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="AB26" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="AC26" s="10" t="s">
+      <c r="AD26" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="AD26" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="AE26" s="10" t="s">
         <v>55</v>
@@ -3377,28 +3374,28 @@
     </row>
     <row r="27" spans="1:32" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>217</v>
-      </c>
       <c r="H27" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>32</v>
@@ -3410,7 +3407,7 @@
         <v>40</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M27" s="7" t="s">
         <v>42</v>
@@ -3428,13 +3425,13 @@
         <v>44</v>
       </c>
       <c r="R27" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="S27" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="S27" s="7" t="s">
+      <c r="T27" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="T27" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="U27" s="7" t="s">
         <v>69</v>
@@ -3452,19 +3449,19 @@
         <v>51</v>
       </c>
       <c r="Z27" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA27" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="AA27" s="7" t="s">
+      <c r="AB27" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AC27" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="AB27" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="AC27" s="6" t="s">
+      <c r="AD27" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="AD27" s="6" t="s">
-        <v>225</v>
       </c>
       <c r="AE27" s="6" t="s">
         <v>55</v>
@@ -3473,30 +3470,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:32" ht="45" customHeight="1">
+    <row r="28" spans="1:32" ht="60" customHeight="1">
       <c r="A28" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>226</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>227</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>116</v>
       </c>
       <c r="E28" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="F28" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>229</v>
-      </c>
       <c r="H28" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>32</v>
@@ -3526,13 +3523,13 @@
         <v>44</v>
       </c>
       <c r="R28" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="S28" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="S28" s="11" t="s">
+      <c r="T28" s="11" t="s">
         <v>231</v>
-      </c>
-      <c r="T28" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="U28" s="11" t="s">
         <v>69</v>
@@ -3550,19 +3547,19 @@
         <v>51</v>
       </c>
       <c r="Z28" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="AA28" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="AA28" s="11" t="s">
+      <c r="AB28" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC28" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="AB28" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="AC28" s="10" t="s">
+      <c r="AD28" s="10" t="s">
         <v>235</v>
-      </c>
-      <c r="AD28" s="10" t="s">
-        <v>236</v>
       </c>
       <c r="AE28" s="10" t="s">
         <v>55</v>
@@ -3573,28 +3570,28 @@
     </row>
     <row r="29" spans="1:32" ht="60" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E29" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G29" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="H29" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>32</v>
@@ -3624,13 +3621,13 @@
         <v>44</v>
       </c>
       <c r="R29" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="S29" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="S29" s="7" t="s">
+      <c r="T29" s="7" t="s">
         <v>242</v>
-      </c>
-      <c r="T29" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="U29" s="7" t="s">
         <v>69</v>
@@ -3648,19 +3645,19 @@
         <v>51</v>
       </c>
       <c r="Z29" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="AA29" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="AA29" s="7" t="s">
+      <c r="AB29" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="AC29" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="AB29" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="AC29" s="6" t="s">
-        <v>246</v>
-      </c>
       <c r="AD29" s="6" t="s">
-        <v>236</v>
+        <v>166</v>
       </c>
       <c r="AE29" s="6" t="s">
         <v>55</v>
@@ -3671,28 +3668,28 @@
     </row>
     <row r="30" spans="1:32">
       <c r="A30" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="C30" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="E30" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="F30" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="G30" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>253</v>
-      </c>
       <c r="H30" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>32</v>
@@ -3704,7 +3701,7 @@
         <v>40</v>
       </c>
       <c r="L30" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M30" s="11" t="s">
         <v>42</v>
@@ -3722,13 +3719,13 @@
         <v>44</v>
       </c>
       <c r="R30" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="S30" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="S30" s="11" t="s">
+      <c r="T30" s="11" t="s">
         <v>256</v>
-      </c>
-      <c r="T30" s="11" t="s">
-        <v>257</v>
       </c>
       <c r="U30" s="11" t="s">
         <v>83</v>
@@ -3746,19 +3743,19 @@
         <v>51</v>
       </c>
       <c r="Z30" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA30" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="AA30" s="11" t="s">
+      <c r="AB30" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="AC30" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="AB30" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="AC30" s="10" t="s">
+      <c r="AD30" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="AD30" s="10" t="s">
-        <v>261</v>
       </c>
       <c r="AE30" s="10" t="s">
         <v>55</v>
@@ -3790,27 +3787,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>